<commit_message>
Fixed errors on script petrobras_1b
</commit_message>
<xml_diff>
--- a/services/petrobras_1b/input/leilao 04.2020.xlsx
+++ b/services/petrobras_1b/input/leilao 04.2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aigm\Desktop\ALIENACAO\2020\FASE 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\ma_digitalization\services\petrobras_1b\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6FE9B25-B06E-4B76-BEAA-13A4AA0059C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B233BF9-FBD6-464A-9F55-124F13AAA065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Materiais" sheetId="1" r:id="rId1"/>
@@ -1193,10 +1193,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1205,19 +1205,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="3" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1257,12 +1257,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="65" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="65" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="16" fillId="3" borderId="8" xfId="65" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1274,9 +1268,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1292,7 +1284,7 @@
     <xf numFmtId="0" fontId="15" fillId="50" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Accent1 - 20%" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1313,6 +1305,7 @@
     <cellStyle name="Accent6 - 20%" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Accent6 - 40%" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Accent6 - 60%" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Comma" xfId="65" builtinId="3"/>
     <cellStyle name="Emphasis 1" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Emphasis 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Emphasis 3" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
@@ -1360,7 +1353,6 @@
     <cellStyle name="SAPBEXunassignedItem" xfId="62" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
     <cellStyle name="SAPBEXundefined" xfId="63" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
     <cellStyle name="Sheet Title" xfId="64" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Vírgula" xfId="65" builtinId="3"/>
   </cellStyles>
   <dxfs count="25">
     <dxf>
@@ -23321,9 +23313,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
@@ -23339,7 +23331,7 @@
     <col min="7" max="7" width="5.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="29" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" style="5" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="11"/>
@@ -23350,25 +23342,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="42"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -23398,7 +23390,7 @@
       <c r="I2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="27" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="10" t="s">
@@ -23427,10 +23419,10 @@
       <c r="B3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="2">
         <v>84821010</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="2">
         <v>31171504</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -23439,7 +23431,7 @@
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H3" s="7" t="s">
@@ -23448,7 +23440,7 @@
       <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="28">
         <v>4</v>
       </c>
       <c r="K3" s="8">
@@ -23457,10 +23449,10 @@
       <c r="L3" s="9">
         <v>292</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="12">
         <v>64</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O3" s="12">
@@ -23468,7 +23460,7 @@
         <v>1</v>
       </c>
       <c r="P3" s="1" t="str">
-        <f>M3&amp;A3</f>
+        <f t="shared" ref="P3:P39" si="1">M3&amp;A3</f>
         <v>6410016642</v>
       </c>
     </row>
@@ -23479,10 +23471,10 @@
       <c r="B4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="2">
         <v>84821010</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="2">
         <v>31171504</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -23491,7 +23483,7 @@
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -23500,7 +23492,7 @@
       <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="28">
         <v>1</v>
       </c>
       <c r="K4" s="8">
@@ -23509,10 +23501,10 @@
       <c r="L4" s="9">
         <v>951</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="12">
         <v>64</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O4" s="12">
@@ -23520,7 +23512,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="1" t="str">
-        <f>M4&amp;A4</f>
+        <f t="shared" si="1"/>
         <v>6410016762</v>
       </c>
     </row>
@@ -23531,10 +23523,10 @@
       <c r="B5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="2">
         <v>84825010</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="2">
         <v>31171505</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -23543,7 +23535,7 @@
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -23552,7 +23544,7 @@
       <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="28">
         <v>1</v>
       </c>
       <c r="K5" s="8">
@@ -23561,10 +23553,10 @@
       <c r="L5" s="9">
         <v>325.25</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="12">
         <v>64</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O5" s="12">
@@ -23572,7 +23564,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="1" t="str">
-        <f>M5&amp;A5</f>
+        <f t="shared" si="1"/>
         <v>6410018461</v>
       </c>
     </row>
@@ -23583,7 +23575,7 @@
       <c r="B6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="2">
         <v>40169300</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -23595,7 +23587,7 @@
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -23604,7 +23596,7 @@
       <c r="I6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="28">
         <v>1</v>
       </c>
       <c r="K6" s="8">
@@ -23613,10 +23605,10 @@
       <c r="L6" s="9">
         <v>85.51</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="12">
         <v>64</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O6" s="12">
@@ -23624,7 +23616,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="1" t="str">
-        <f>M6&amp;A6</f>
+        <f t="shared" si="1"/>
         <v>6410020074</v>
       </c>
     </row>
@@ -23635,7 +23627,7 @@
       <c r="B7" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="2">
         <v>81019990</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -23647,7 +23639,7 @@
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -23656,7 +23648,7 @@
       <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="28">
         <v>1</v>
       </c>
       <c r="K7" s="8">
@@ -23665,10 +23657,10 @@
       <c r="L7" s="9">
         <v>0</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="12">
         <v>64</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O7" s="12">
@@ -23676,7 +23668,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="1" t="str">
-        <f>M7&amp;A7</f>
+        <f t="shared" si="1"/>
         <v>6410020383</v>
       </c>
     </row>
@@ -23687,7 +23679,7 @@
       <c r="B8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="2">
         <v>68151090</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -23699,7 +23691,7 @@
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -23708,7 +23700,7 @@
       <c r="I8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="28">
         <v>1</v>
       </c>
       <c r="K8" s="8">
@@ -23717,10 +23709,10 @@
       <c r="L8" s="9">
         <v>1349.48</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="12">
         <v>64</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O8" s="12">
@@ -23728,7 +23720,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="1" t="str">
-        <f>M8&amp;A8</f>
+        <f t="shared" si="1"/>
         <v>6410020529</v>
       </c>
     </row>
@@ -23739,7 +23731,7 @@
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="2">
         <v>81019990</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -23751,7 +23743,7 @@
       <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -23760,7 +23752,7 @@
       <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="28">
         <v>9</v>
       </c>
       <c r="K9" s="8">
@@ -23769,10 +23761,10 @@
       <c r="L9" s="9">
         <v>0</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="12">
         <v>64</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O9" s="12">
@@ -23780,7 +23772,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="1" t="str">
-        <f>M9&amp;A9</f>
+        <f t="shared" si="1"/>
         <v>6410020585</v>
       </c>
     </row>
@@ -23791,7 +23783,7 @@
       <c r="B10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="2">
         <v>68151090</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -23803,7 +23795,7 @@
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -23812,7 +23804,7 @@
       <c r="I10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="28">
         <v>1</v>
       </c>
       <c r="K10" s="8">
@@ -23821,10 +23813,10 @@
       <c r="L10" s="9">
         <v>973.99</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="12">
         <v>64</v>
       </c>
-      <c r="N10" s="25" t="s">
+      <c r="N10" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O10" s="12">
@@ -23832,7 +23824,7 @@
         <v>1</v>
       </c>
       <c r="P10" s="1" t="str">
-        <f>M10&amp;A10</f>
+        <f t="shared" si="1"/>
         <v>6410020624</v>
       </c>
     </row>
@@ -23843,7 +23835,7 @@
       <c r="B11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="2">
         <v>81019990</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -23855,7 +23847,7 @@
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -23864,7 +23856,7 @@
       <c r="I11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="28">
         <v>7</v>
       </c>
       <c r="K11" s="8">
@@ -23873,10 +23865,10 @@
       <c r="L11" s="9">
         <v>0</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="12">
         <v>64</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O11" s="12">
@@ -23884,7 +23876,7 @@
         <v>1</v>
       </c>
       <c r="P11" s="1" t="str">
-        <f>M11&amp;A11</f>
+        <f t="shared" si="1"/>
         <v>6410020676</v>
       </c>
     </row>
@@ -23895,7 +23887,7 @@
       <c r="B12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="2">
         <v>73269090</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -23907,7 +23899,7 @@
       <c r="F12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H12" s="7" t="s">
@@ -23916,7 +23908,7 @@
       <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J12" s="28">
         <v>5</v>
       </c>
       <c r="K12" s="8">
@@ -23925,10 +23917,10 @@
       <c r="L12" s="9">
         <v>331.92</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="12">
         <v>64</v>
       </c>
-      <c r="N12" s="25" t="s">
+      <c r="N12" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O12" s="12">
@@ -23936,7 +23928,7 @@
         <v>1</v>
       </c>
       <c r="P12" s="1" t="str">
-        <f>M12&amp;A12</f>
+        <f t="shared" si="1"/>
         <v>6410020736</v>
       </c>
     </row>
@@ -23947,10 +23939,10 @@
       <c r="B13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="2">
         <v>68151090</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -23959,7 +23951,7 @@
       <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -23968,7 +23960,7 @@
       <c r="I13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J13" s="28">
         <v>3</v>
       </c>
       <c r="K13" s="8">
@@ -23977,10 +23969,10 @@
       <c r="L13" s="9">
         <v>0</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="12">
         <v>64</v>
       </c>
-      <c r="N13" s="25" t="s">
+      <c r="N13" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O13" s="12">
@@ -23988,7 +23980,7 @@
         <v>1</v>
       </c>
       <c r="P13" s="1" t="str">
-        <f>M13&amp;A13</f>
+        <f t="shared" si="1"/>
         <v>6410020931</v>
       </c>
     </row>
@@ -23999,10 +23991,10 @@
       <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="2">
         <v>81019990</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -24011,7 +24003,7 @@
       <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -24020,7 +24012,7 @@
       <c r="I14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="28">
         <v>48</v>
       </c>
       <c r="K14" s="8">
@@ -24029,10 +24021,10 @@
       <c r="L14" s="9">
         <v>0</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="12">
         <v>64</v>
       </c>
-      <c r="N14" s="25" t="s">
+      <c r="N14" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O14" s="12">
@@ -24040,7 +24032,7 @@
         <v>1</v>
       </c>
       <c r="P14" s="1" t="str">
-        <f>M14&amp;A14</f>
+        <f t="shared" si="1"/>
         <v>6410020994</v>
       </c>
     </row>
@@ -24051,10 +24043,10 @@
       <c r="B15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="2">
         <v>69091990</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -24063,7 +24055,7 @@
       <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H15" s="7" t="s">
@@ -24072,7 +24064,7 @@
       <c r="I15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="30">
+      <c r="J15" s="28">
         <v>4</v>
       </c>
       <c r="K15" s="8">
@@ -24081,10 +24073,10 @@
       <c r="L15" s="9">
         <v>2131.94</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="12">
         <v>64</v>
       </c>
-      <c r="N15" s="25" t="s">
+      <c r="N15" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O15" s="12">
@@ -24092,7 +24084,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="1" t="str">
-        <f>M15&amp;A15</f>
+        <f t="shared" si="1"/>
         <v>6410061943</v>
       </c>
     </row>
@@ -24103,10 +24095,10 @@
       <c r="B16" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="2">
         <v>84139190</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -24124,7 +24116,7 @@
       <c r="I16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="28">
         <v>1</v>
       </c>
       <c r="K16" s="8">
@@ -24133,10 +24125,10 @@
       <c r="L16" s="9">
         <v>58261.71</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="12">
         <v>64</v>
       </c>
-      <c r="N16" s="25" t="s">
+      <c r="N16" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O16" s="12">
@@ -24144,7 +24136,7 @@
         <v>0.5</v>
       </c>
       <c r="P16" s="1" t="str">
-        <f>M16&amp;A16</f>
+        <f t="shared" si="1"/>
         <v>6410093133</v>
       </c>
     </row>
@@ -24155,7 +24147,7 @@
       <c r="B17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="2">
         <v>84139190</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -24167,7 +24159,7 @@
       <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H17" s="7" t="s">
@@ -24176,7 +24168,7 @@
       <c r="I17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="30">
+      <c r="J17" s="28">
         <v>1</v>
       </c>
       <c r="K17" s="8">
@@ -24185,10 +24177,10 @@
       <c r="L17" s="9">
         <v>58261.71</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="12">
         <v>64</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="N17" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O17" s="12">
@@ -24196,7 +24188,7 @@
         <v>0.5</v>
       </c>
       <c r="P17" s="1" t="str">
-        <f>M17&amp;A17</f>
+        <f t="shared" si="1"/>
         <v>6410093133</v>
       </c>
     </row>
@@ -24207,7 +24199,7 @@
       <c r="B18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="2">
         <v>73269090</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -24219,7 +24211,7 @@
       <c r="F18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H18" s="7" t="s">
@@ -24228,7 +24220,7 @@
       <c r="I18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="30">
+      <c r="J18" s="28">
         <v>1</v>
       </c>
       <c r="K18" s="8">
@@ -24237,10 +24229,10 @@
       <c r="L18" s="9">
         <v>0.01</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="12">
         <v>64</v>
       </c>
-      <c r="N18" s="25" t="s">
+      <c r="N18" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O18" s="12">
@@ -24248,7 +24240,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1" t="str">
-        <f>M18&amp;A18</f>
+        <f t="shared" si="1"/>
         <v>6410287048</v>
       </c>
     </row>
@@ -24259,7 +24251,7 @@
       <c r="B19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="2">
         <v>84819090</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -24271,7 +24263,7 @@
       <c r="F19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H19" s="7" t="s">
@@ -24280,7 +24272,7 @@
       <c r="I19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="30">
+      <c r="J19" s="28">
         <v>1</v>
       </c>
       <c r="K19" s="8">
@@ -24289,10 +24281,10 @@
       <c r="L19" s="9">
         <v>10</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="12">
         <v>65</v>
       </c>
-      <c r="N19" s="25" t="s">
+      <c r="N19" s="12" t="s">
         <v>125</v>
       </c>
       <c r="O19" s="12">
@@ -24300,7 +24292,7 @@
         <v>1</v>
       </c>
       <c r="P19" s="1" t="str">
-        <f>M19&amp;A19</f>
+        <f t="shared" si="1"/>
         <v>6510293473</v>
       </c>
     </row>
@@ -24311,7 +24303,7 @@
       <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="2">
         <v>90318099</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -24323,7 +24315,7 @@
       <c r="F20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="7" t="s">
@@ -24332,7 +24324,7 @@
       <c r="I20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="28">
         <v>1</v>
       </c>
       <c r="K20" s="8">
@@ -24341,10 +24333,10 @@
       <c r="L20" s="9">
         <v>0.2</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="12">
         <v>64</v>
       </c>
-      <c r="N20" s="25" t="s">
+      <c r="N20" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O20" s="12">
@@ -24352,7 +24344,7 @@
         <v>1</v>
       </c>
       <c r="P20" s="1" t="str">
-        <f>M20&amp;A20</f>
+        <f t="shared" si="1"/>
         <v>6410327403</v>
       </c>
     </row>
@@ -24363,10 +24355,10 @@
       <c r="B21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="2">
         <v>84836090</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="2">
         <v>31163002</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -24375,7 +24367,7 @@
       <c r="F21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H21" s="7" t="s">
@@ -24384,7 +24376,7 @@
       <c r="I21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="30">
+      <c r="J21" s="28">
         <v>3</v>
       </c>
       <c r="K21" s="8">
@@ -24393,10 +24385,10 @@
       <c r="L21" s="9">
         <v>1182.79</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="12">
         <v>64</v>
       </c>
-      <c r="N21" s="25" t="s">
+      <c r="N21" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O21" s="12">
@@ -24404,7 +24396,7 @@
         <v>1</v>
       </c>
       <c r="P21" s="1" t="str">
-        <f>M21&amp;A21</f>
+        <f t="shared" si="1"/>
         <v>6410591493</v>
       </c>
     </row>
@@ -24415,10 +24407,10 @@
       <c r="B22" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="2">
         <v>84839000</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -24427,7 +24419,7 @@
       <c r="F22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H22" s="7" t="s">
@@ -24436,7 +24428,7 @@
       <c r="I22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="30">
+      <c r="J22" s="28">
         <v>1</v>
       </c>
       <c r="K22" s="8">
@@ -24445,10 +24437,10 @@
       <c r="L22" s="9">
         <v>1</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="12">
         <v>64</v>
       </c>
-      <c r="N22" s="25" t="s">
+      <c r="N22" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O22" s="12">
@@ -24456,7 +24448,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="1" t="str">
-        <f>M22&amp;A22</f>
+        <f t="shared" si="1"/>
         <v>6411218886</v>
       </c>
     </row>
@@ -24467,7 +24459,7 @@
       <c r="B23" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="2">
         <v>73181600</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -24479,7 +24471,7 @@
       <c r="F23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H23" s="7" t="s">
@@ -24488,7 +24480,7 @@
       <c r="I23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="30">
+      <c r="J23" s="28">
         <v>13</v>
       </c>
       <c r="K23" s="8">
@@ -24497,10 +24489,10 @@
       <c r="L23" s="9">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23" s="12">
         <v>64</v>
       </c>
-      <c r="N23" s="25" t="s">
+      <c r="N23" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O23" s="12">
@@ -24508,7 +24500,7 @@
         <v>1</v>
       </c>
       <c r="P23" s="1" t="str">
-        <f>M23&amp;A23</f>
+        <f t="shared" si="1"/>
         <v>6411241075</v>
       </c>
     </row>
@@ -24519,7 +24511,7 @@
       <c r="B24" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="2">
         <v>84813000</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -24531,7 +24523,7 @@
       <c r="F24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H24" s="7" t="s">
@@ -24540,7 +24532,7 @@
       <c r="I24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="30">
+      <c r="J24" s="28">
         <v>2</v>
       </c>
       <c r="K24" s="8">
@@ -24549,10 +24541,10 @@
       <c r="L24" s="9">
         <v>2</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24" s="12">
         <v>64</v>
       </c>
-      <c r="N24" s="25" t="s">
+      <c r="N24" s="12" t="s">
         <v>127</v>
       </c>
       <c r="O24" s="12">
@@ -24560,7 +24552,7 @@
         <v>1</v>
       </c>
       <c r="P24" s="1" t="str">
-        <f>M24&amp;A24</f>
+        <f t="shared" si="1"/>
         <v>6411289322</v>
       </c>
     </row>
@@ -24571,10 +24563,10 @@
       <c r="B25" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="2">
         <v>68069090</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="2">
         <v>30141505</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -24583,7 +24575,7 @@
       <c r="F25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H25" s="7" t="s">
@@ -24592,7 +24584,7 @@
       <c r="I25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J25" s="28">
         <v>1</v>
       </c>
       <c r="K25" s="8">
@@ -24601,10 +24593,10 @@
       <c r="L25" s="9">
         <v>17.87</v>
       </c>
-      <c r="M25" s="25">
+      <c r="M25" s="12">
         <v>66</v>
       </c>
-      <c r="N25" s="25" t="s">
+      <c r="N25" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O25" s="12">
@@ -24612,7 +24604,7 @@
         <v>0.5</v>
       </c>
       <c r="P25" s="1" t="str">
-        <f>M25&amp;A25</f>
+        <f t="shared" si="1"/>
         <v>6610037769</v>
       </c>
     </row>
@@ -24623,10 +24615,10 @@
       <c r="B26" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="2">
         <v>68069090</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="2">
         <v>30141505</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -24635,7 +24627,7 @@
       <c r="F26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H26" s="7" t="s">
@@ -24644,7 +24636,7 @@
       <c r="I26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="30">
+      <c r="J26" s="28">
         <v>32</v>
       </c>
       <c r="K26" s="8">
@@ -24653,10 +24645,10 @@
       <c r="L26" s="9">
         <v>571.87559999999996</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="12">
         <v>66</v>
       </c>
-      <c r="N26" s="25" t="s">
+      <c r="N26" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O26" s="12">
@@ -24664,7 +24656,7 @@
         <v>0.5</v>
       </c>
       <c r="P26" s="1" t="str">
-        <f>M26&amp;A26</f>
+        <f t="shared" si="1"/>
         <v>6610037769</v>
       </c>
     </row>
@@ -24675,10 +24667,10 @@
       <c r="B27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="2">
         <v>90262090</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="2">
         <v>41112410</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -24687,7 +24679,7 @@
       <c r="F27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="2" t="s">
         <v>64</v>
       </c>
       <c r="H27" s="7" t="s">
@@ -24696,7 +24688,7 @@
       <c r="I27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="30">
+      <c r="J27" s="28">
         <v>5</v>
       </c>
       <c r="K27" s="8">
@@ -24705,10 +24697,10 @@
       <c r="L27" s="9">
         <v>7409.6733000000004</v>
       </c>
-      <c r="M27" s="25">
+      <c r="M27" s="12">
         <v>67</v>
       </c>
-      <c r="N27" s="25" t="s">
+      <c r="N27" s="12" t="s">
         <v>124</v>
       </c>
       <c r="O27" s="12">
@@ -24716,7 +24708,7 @@
         <v>0.5</v>
       </c>
       <c r="P27" s="1" t="str">
-        <f>M27&amp;A27</f>
+        <f t="shared" si="1"/>
         <v>6710057372</v>
       </c>
     </row>
@@ -24727,10 +24719,10 @@
       <c r="B28" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="2">
         <v>90262090</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="2">
         <v>41112410</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -24739,7 +24731,7 @@
       <c r="F28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="2" t="s">
         <v>64</v>
       </c>
       <c r="H28" s="7" t="s">
@@ -24748,7 +24740,7 @@
       <c r="I28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J28" s="30">
+      <c r="J28" s="28">
         <v>2</v>
       </c>
       <c r="K28" s="8">
@@ -24757,10 +24749,10 @@
       <c r="L28" s="9">
         <v>2963.87</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="12">
         <v>67</v>
       </c>
-      <c r="N28" s="25" t="s">
+      <c r="N28" s="12" t="s">
         <v>124</v>
       </c>
       <c r="O28" s="12">
@@ -24768,7 +24760,7 @@
         <v>0.5</v>
       </c>
       <c r="P28" s="1" t="str">
-        <f>M28&amp;A28</f>
+        <f t="shared" si="1"/>
         <v>6710057372</v>
       </c>
     </row>
@@ -24779,10 +24771,10 @@
       <c r="B29" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="2">
         <v>68069090</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="2">
         <v>30141505</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -24791,7 +24783,7 @@
       <c r="F29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H29" s="7" t="s">
@@ -24800,7 +24792,7 @@
       <c r="I29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J29" s="30">
+      <c r="J29" s="28">
         <v>270</v>
       </c>
       <c r="K29" s="8">
@@ -24809,10 +24801,10 @@
       <c r="L29" s="9">
         <v>3846.69</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="12">
         <v>66</v>
       </c>
-      <c r="N29" s="25" t="s">
+      <c r="N29" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O29" s="12">
@@ -24820,7 +24812,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="P29" s="1" t="str">
-        <f>M29&amp;A29</f>
+        <f t="shared" si="1"/>
         <v>6610176593</v>
       </c>
     </row>
@@ -24831,10 +24823,10 @@
       <c r="B30" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="2">
         <v>68069090</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="2">
         <v>30141505</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -24843,7 +24835,7 @@
       <c r="F30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G30" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H30" s="7" t="s">
@@ -24852,7 +24844,7 @@
       <c r="I30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J30" s="30">
+      <c r="J30" s="28">
         <v>10</v>
       </c>
       <c r="K30" s="8">
@@ -24861,10 +24853,10 @@
       <c r="L30" s="9">
         <v>142.47</v>
       </c>
-      <c r="M30" s="25">
+      <c r="M30" s="12">
         <v>66</v>
       </c>
-      <c r="N30" s="25" t="s">
+      <c r="N30" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O30" s="12">
@@ -24872,7 +24864,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="P30" s="1" t="str">
-        <f>M30&amp;A30</f>
+        <f t="shared" si="1"/>
         <v>6610176593</v>
       </c>
     </row>
@@ -24883,10 +24875,10 @@
       <c r="B31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="2">
         <v>68069090</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="2">
         <v>30141505</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -24895,7 +24887,7 @@
       <c r="F31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="26" t="s">
+      <c r="G31" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H31" s="7" t="s">
@@ -24904,7 +24896,7 @@
       <c r="I31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="30">
+      <c r="J31" s="28">
         <v>1410</v>
       </c>
       <c r="K31" s="8">
@@ -24913,10 +24905,10 @@
       <c r="L31" s="9">
         <v>20088.310000000001</v>
       </c>
-      <c r="M31" s="25">
+      <c r="M31" s="12">
         <v>66</v>
       </c>
-      <c r="N31" s="25" t="s">
+      <c r="N31" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O31" s="12">
@@ -24924,7 +24916,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="P31" s="1" t="str">
-        <f>M31&amp;A31</f>
+        <f t="shared" si="1"/>
         <v>6610176593</v>
       </c>
     </row>
@@ -24935,10 +24927,10 @@
       <c r="B32" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="2">
         <v>73182200</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="7" t="s">
@@ -24947,7 +24939,7 @@
       <c r="F32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="26" t="s">
+      <c r="G32" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H32" s="7" t="s">
@@ -24956,7 +24948,7 @@
       <c r="I32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="30">
+      <c r="J32" s="28">
         <v>1000</v>
       </c>
       <c r="K32" s="8">
@@ -24965,10 +24957,10 @@
       <c r="L32" s="9">
         <v>1606.31</v>
       </c>
-      <c r="M32" s="25">
+      <c r="M32" s="12">
         <v>65</v>
       </c>
-      <c r="N32" s="25" t="s">
+      <c r="N32" s="12" t="s">
         <v>125</v>
       </c>
       <c r="O32" s="12">
@@ -24976,7 +24968,7 @@
         <v>0.25</v>
       </c>
       <c r="P32" s="1" t="str">
-        <f>M32&amp;A32</f>
+        <f t="shared" si="1"/>
         <v>6510216905</v>
       </c>
     </row>
@@ -24987,10 +24979,10 @@
       <c r="B33" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="2">
         <v>73182200</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E33" s="7" t="s">
@@ -24999,7 +24991,7 @@
       <c r="F33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="26" t="s">
+      <c r="G33" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H33" s="7" t="s">
@@ -25008,7 +25000,7 @@
       <c r="I33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J33" s="30">
+      <c r="J33" s="28">
         <v>1000</v>
       </c>
       <c r="K33" s="8">
@@ -25017,10 +25009,10 @@
       <c r="L33" s="9">
         <v>2846.01</v>
       </c>
-      <c r="M33" s="25">
+      <c r="M33" s="12">
         <v>65</v>
       </c>
-      <c r="N33" s="25" t="s">
+      <c r="N33" s="12" t="s">
         <v>125</v>
       </c>
       <c r="O33" s="12">
@@ -25028,7 +25020,7 @@
         <v>0.25</v>
       </c>
       <c r="P33" s="1" t="str">
-        <f>M33&amp;A33</f>
+        <f t="shared" si="1"/>
         <v>6510216905</v>
       </c>
     </row>
@@ -25039,10 +25031,10 @@
       <c r="B34" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="2">
         <v>73182200</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -25051,7 +25043,7 @@
       <c r="F34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H34" s="7" t="s">
@@ -25060,7 +25052,7 @@
       <c r="I34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="30">
+      <c r="J34" s="28">
         <v>900</v>
       </c>
       <c r="K34" s="8">
@@ -25069,10 +25061,10 @@
       <c r="L34" s="9">
         <v>2561.41</v>
       </c>
-      <c r="M34" s="25">
+      <c r="M34" s="12">
         <v>65</v>
       </c>
-      <c r="N34" s="25" t="s">
+      <c r="N34" s="12" t="s">
         <v>125</v>
       </c>
       <c r="O34" s="12">
@@ -25080,7 +25072,7 @@
         <v>0.25</v>
       </c>
       <c r="P34" s="1" t="str">
-        <f>M34&amp;A34</f>
+        <f t="shared" si="1"/>
         <v>6510216905</v>
       </c>
     </row>
@@ -25091,10 +25083,10 @@
       <c r="B35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="2">
         <v>73182200</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -25103,7 +25095,7 @@
       <c r="F35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -25112,7 +25104,7 @@
       <c r="I35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J35" s="30">
+      <c r="J35" s="28">
         <v>900</v>
       </c>
       <c r="K35" s="8">
@@ -25121,10 +25113,10 @@
       <c r="L35" s="9">
         <v>3208.527</v>
       </c>
-      <c r="M35" s="25">
+      <c r="M35" s="12">
         <v>65</v>
       </c>
-      <c r="N35" s="25" t="s">
+      <c r="N35" s="12" t="s">
         <v>125</v>
       </c>
       <c r="O35" s="12">
@@ -25132,7 +25124,7 @@
         <v>0.25</v>
       </c>
       <c r="P35" s="1" t="str">
-        <f>M35&amp;A35</f>
+        <f t="shared" si="1"/>
         <v>6510216905</v>
       </c>
     </row>
@@ -25143,10 +25135,10 @@
       <c r="B36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="2">
         <v>94051093</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -25155,7 +25147,7 @@
       <c r="F36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="26" t="s">
+      <c r="G36" s="2" t="s">
         <v>64</v>
       </c>
       <c r="H36" s="7" t="s">
@@ -25164,7 +25156,7 @@
       <c r="I36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J36" s="30">
+      <c r="J36" s="28">
         <v>10</v>
       </c>
       <c r="K36" s="8">
@@ -25173,10 +25165,10 @@
       <c r="L36" s="9">
         <v>658.4</v>
       </c>
-      <c r="M36" s="25">
+      <c r="M36" s="12">
         <v>66</v>
       </c>
-      <c r="N36" s="25" t="s">
+      <c r="N36" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O36" s="12">
@@ -25184,7 +25176,7 @@
         <v>0.5</v>
       </c>
       <c r="P36" s="1" t="str">
-        <f>M36&amp;A36</f>
+        <f t="shared" si="1"/>
         <v>6610262047</v>
       </c>
     </row>
@@ -25195,10 +25187,10 @@
       <c r="B37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="2">
         <v>94051093</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -25207,7 +25199,7 @@
       <c r="F37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="H37" s="7" t="s">
@@ -25216,7 +25208,7 @@
       <c r="I37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J37" s="30">
+      <c r="J37" s="28">
         <v>5</v>
       </c>
       <c r="K37" s="8">
@@ -25225,10 +25217,10 @@
       <c r="L37" s="9">
         <v>329.2</v>
       </c>
-      <c r="M37" s="25">
+      <c r="M37" s="12">
         <v>66</v>
       </c>
-      <c r="N37" s="25" t="s">
+      <c r="N37" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O37" s="12">
@@ -25236,7 +25228,7 @@
         <v>0.5</v>
       </c>
       <c r="P37" s="1" t="str">
-        <f>M37&amp;A37</f>
+        <f t="shared" si="1"/>
         <v>6610262047</v>
       </c>
     </row>
@@ -25247,10 +25239,10 @@
       <c r="B38" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="2">
         <v>68069090</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="2">
         <v>30141507</v>
       </c>
       <c r="E38" s="7" t="s">
@@ -25259,7 +25251,7 @@
       <c r="F38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="26" t="s">
+      <c r="G38" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H38" s="7" t="s">
@@ -25268,7 +25260,7 @@
       <c r="I38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J38" s="30">
+      <c r="J38" s="28">
         <v>10</v>
       </c>
       <c r="K38" s="8">
@@ -25277,10 +25269,10 @@
       <c r="L38" s="9">
         <v>321.89</v>
       </c>
-      <c r="M38" s="25">
+      <c r="M38" s="12">
         <v>66</v>
       </c>
-      <c r="N38" s="25" t="s">
+      <c r="N38" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O38" s="12">
@@ -25288,7 +25280,7 @@
         <v>0.5</v>
       </c>
       <c r="P38" s="1" t="str">
-        <f>M38&amp;A38</f>
+        <f t="shared" si="1"/>
         <v>6610280847</v>
       </c>
     </row>
@@ -25299,10 +25291,10 @@
       <c r="B39" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="2">
         <v>68069090</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="2">
         <v>30141507</v>
       </c>
       <c r="E39" s="7" t="s">
@@ -25311,7 +25303,7 @@
       <c r="F39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G39" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H39" s="7" t="s">
@@ -25320,7 +25312,7 @@
       <c r="I39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J39" s="30">
+      <c r="J39" s="28">
         <v>428</v>
       </c>
       <c r="K39" s="8">
@@ -25329,10 +25321,10 @@
       <c r="L39" s="9">
         <v>13777.093699999999</v>
       </c>
-      <c r="M39" s="25">
+      <c r="M39" s="12">
         <v>66</v>
       </c>
-      <c r="N39" s="25" t="s">
+      <c r="N39" s="12" t="s">
         <v>126</v>
       </c>
       <c r="O39" s="12">
@@ -25340,7 +25332,7 @@
         <v>0.5</v>
       </c>
       <c r="P39" s="1" t="str">
-        <f>M39&amp;A39</f>
+        <f t="shared" si="1"/>
         <v>6610280847</v>
       </c>
     </row>
@@ -25364,9 +25356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25472,14 +25464,10 @@
         <f t="shared" ref="I4:I9" si="0">IF(ISERR(H4/G4),"-",H4/G4)</f>
         <v>2.3641893384257241E-2</v>
       </c>
-      <c r="J4" s="22" t="str">
-        <f t="shared" ref="J4:J9" si="1">IF(I4&gt;=0.4,0.05*G4,IF(I4&gt;=0.05,0.01*G4,"Sucata ou aplicar 1%"))</f>
-        <v>Sucata ou aplicar 1%</v>
-      </c>
-      <c r="K4" s="43">
-        <f>G4*1%</f>
-        <v>102.32260000000001</v>
-      </c>
+      <c r="J4" s="39">
+        <v>102.32</v>
+      </c>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
@@ -25508,7 +25496,7 @@
         <v>7.1605733288390039E-2</v>
       </c>
       <c r="J5" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J4:J9" si="1">IF(I5&gt;=0.4,0.05*G5,IF(I5&gt;=0.05,0.01*G5,"Sucata ou aplicar 1%"))</f>
         <v>397.53800000000001</v>
       </c>
     </row>
@@ -25655,13 +25643,13 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="31" t="s">
         <v>40</v>
       </c>
       <c r="F3"/>
@@ -25680,7 +25668,7 @@
       <c r="D4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>41</v>
       </c>
       <c r="F4" t="s">
@@ -25703,13 +25691,13 @@
       <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="30">
         <v>21</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="32">
         <v>124169.70999999999</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <v>133352.61434430841</v>
       </c>
     </row>
@@ -25726,13 +25714,13 @@
       <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="30">
         <v>127.16666666666667</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>307652.1324</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="32">
         <v>59808.59121037522</v>
       </c>
     </row>
@@ -25749,13 +25737,13 @@
       <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="30">
         <v>256.83333333333331</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="32">
         <v>886548.15069999988</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="32">
         <v>382722.75441399351</v>
       </c>
     </row>
@@ -25772,82 +25760,82 @@
       <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="30">
         <v>51</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="32">
         <v>157185.63410000011</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="32">
         <v>89298.827145587013</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="30">
         <v>5</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="32">
         <v>10428.1</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="32">
         <v>20510.637969346139</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="30">
         <v>5</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="32">
         <v>91947.623076923075</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="32">
         <v>8745.6251079301055</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="30">
         <v>1</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="32">
         <v>7650.32</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="32">
         <v>94.055636926287079</v>
       </c>
     </row>
@@ -25864,13 +25852,13 @@
       <c r="D12" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="30">
         <v>56</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="32">
         <v>5499545.1900000023</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="32">
         <v>1694508.1544700004</v>
       </c>
     </row>
@@ -25878,13 +25866,13 @@
       <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="30">
         <v>523</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="32">
         <v>7085126.8602769254</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="32">
         <v>2389041.2602984672</v>
       </c>
     </row>

</xml_diff>